<commit_message>
Update ARS data to include latest report.
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="22">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">From here from 2021-02-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-02-23</t>
   </si>
   <si>
     <t xml:space="preserve">Länge für Einheit (cm)</t>
@@ -272,15 +275,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J168"/>
+  <dimension ref="A1:J180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E80" activeCellId="0" sqref="E80"/>
+      <selection pane="bottomLeft" activeCell="E176" activeCellId="0" sqref="E176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -3241,13 +3244,6 @@
       <c r="G149" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I149" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J149" s="0" t="n">
-        <f aca="false">26-8.9</f>
-        <v>17.1</v>
-      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
@@ -3271,12 +3267,6 @@
       <c r="G150" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="I150" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J150" s="0" t="n">
-        <v>150</v>
-      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
@@ -3300,13 +3290,6 @@
       <c r="G151" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="I151" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J151" s="0" t="n">
-        <f aca="false">J150 / J149</f>
-        <v>8.7719298245614</v>
-      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
@@ -3330,12 +3313,6 @@
       <c r="G152" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="I152" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J152" s="0" t="n">
-        <v>26</v>
-      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
@@ -3359,12 +3336,6 @@
       <c r="G153" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="I153" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J153" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
@@ -3388,21 +3359,6 @@
       <c r="G154" s="0" t="n">
         <v>173</v>
       </c>
-      <c r="I154" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J154" s="3" t="n">
-        <v>18.1</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I155" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J155" s="1" t="n">
-        <f aca="false">(J154-J152)*J151+J153</f>
-        <v>130.701754385965</v>
-      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
@@ -3472,10 +3428,6 @@
       <c r="G158" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="I158" s="0" t="n">
-        <f aca="false">50000/55</f>
-        <v>909.090909090909</v>
-      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
@@ -3499,10 +3451,6 @@
       <c r="G159" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="I159" s="0" t="n">
-        <f aca="false">50000 + 909 * 9</f>
-        <v>58181</v>
-      </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
@@ -3526,10 +3474,6 @@
       <c r="G160" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="I160" s="0" t="n">
-        <f aca="false">909*8</f>
-        <v>7272</v>
-      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
@@ -3690,6 +3634,176 @@
       </c>
       <c r="G168" s="0" t="n">
         <v>130</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I169" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J169" s="0" t="n">
+        <f aca="false">26.4-6</f>
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>7819</v>
+      </c>
+      <c r="E170" s="0" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="I170" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J170" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B171" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" s="0" t="n">
+        <v>10664</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="I171" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J171" s="0" t="n">
+        <f aca="false">J170 / J169</f>
+        <v>0.490196078431373</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B172" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>95972</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="I172" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J172" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>153555</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="I173" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J173" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>86730</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="I174" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J174" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D175" s="0" t="n">
+        <v>53318</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J175" s="1" t="n">
+        <f aca="false">(J174-J172)*J171+J173</f>
+        <v>6.47058823529412</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I178" s="0" t="n">
+        <f aca="false">50000/55</f>
+        <v>909.090909090909</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I179" s="0" t="n">
+        <f aca="false">50000 + 909 * 9</f>
+        <v>58181</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I180" s="0" t="n">
+        <f aca="false">909*8</f>
+        <v>7272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement emergency schooling (#26)
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="23">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-03-02</t>
   </si>
 </sst>
 </file>
@@ -275,15 +278,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J180"/>
+  <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E176" activeCellId="0" sqref="E176"/>
+      <selection pane="bottomLeft" activeCell="J171" activeCellId="0" sqref="J171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -3644,8 +3647,7 @@
         <v>15</v>
       </c>
       <c r="J169" s="0" t="n">
-        <f aca="false">26.4-6</f>
-        <v>20.4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,7 +3670,7 @@
         <v>16</v>
       </c>
       <c r="J170" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3692,7 +3694,7 @@
       </c>
       <c r="J171" s="0" t="n">
         <f aca="false">J170 / J169</f>
-        <v>0.490196078431373</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3715,7 +3717,7 @@
         <v>18</v>
       </c>
       <c r="J172" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3761,7 +3763,7 @@
         <v>20</v>
       </c>
       <c r="J174" s="3" t="n">
-        <v>9</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3785,25 +3787,114 @@
       </c>
       <c r="J175" s="1" t="n">
         <f aca="false">(J174-J172)*J171+J173</f>
-        <v>6.47058823529412</v>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B176" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B177" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="E177" s="0" t="n">
+        <v>6.3</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I178" s="0" t="n">
-        <f aca="false">50000/55</f>
-        <v>909.090909090909</v>
+      <c r="A178" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D178" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E178" s="0" t="n">
+        <v>9.3</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I179" s="0" t="n">
-        <f aca="false">50000 + 909 * 9</f>
-        <v>58181</v>
+      <c r="A179" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>89000</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>5.8</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I180" s="0" t="n">
-        <f aca="false">909*8</f>
-        <v>7272</v>
+      <c r="A180" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B180" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D180" s="0" t="n">
+        <v>143000</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D181" s="0" t="n">
+        <v>80500</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C182" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>53000</v>
+      </c>
+      <c r="E182" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add latest ARS data.
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="24">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Source: 2021-03-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-03-09</t>
   </si>
 </sst>
 </file>
@@ -278,15 +281,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J182"/>
+  <dimension ref="A1:J189"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J171" activeCellId="0" sqref="J171"/>
+      <selection pane="bottomLeft" activeCell="H175" activeCellId="0" sqref="H175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -3647,7 +3650,7 @@
         <v>15</v>
       </c>
       <c r="J169" s="0" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,7 +3697,7 @@
       </c>
       <c r="J171" s="0" t="n">
         <f aca="false">J170 / J169</f>
-        <v>0.333333333333333</v>
+        <v>0.384615384615385</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3763,7 +3766,7 @@
         <v>20</v>
       </c>
       <c r="J174" s="3" t="n">
-        <v>3.6</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,7 +3790,7 @@
       </c>
       <c r="J175" s="1" t="n">
         <f aca="false">(J174-J172)*J171+J173</f>
-        <v>6.2</v>
+        <v>9.42307692307692</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3895,6 +3898,113 @@
       </c>
       <c r="E182" s="0" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B183" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D184" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="E184" s="0" t="n">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D185" s="0" t="n">
+        <v>11250</v>
+      </c>
+      <c r="E185" s="0" t="n">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C186" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D186" s="0" t="n">
+        <v>93750</v>
+      </c>
+      <c r="E186" s="0" t="n">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C187" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>150000</v>
+      </c>
+      <c r="E187" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C188" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D188" s="0" t="n">
+        <v>84750</v>
+      </c>
+      <c r="E188" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C189" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D189" s="0" t="n">
+        <v>46500</v>
+      </c>
+      <c r="E189" s="0" t="n">
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update two weeks of ARS testing data.
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="25">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -67,6 +67,12 @@
     <t xml:space="preserve">Source: 2021-02-23</t>
   </si>
   <si>
+    <t xml:space="preserve">Source: 2021-03-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-03-09</t>
+  </si>
+  <si>
     <t xml:space="preserve">Länge für Einheit (cm)</t>
   </si>
   <si>
@@ -85,13 +91,10 @@
     <t xml:space="preserve">Gemessene Höhe (cm)</t>
   </si>
   <si>
-    <t xml:space="preserve">Zahl</t>
+    <t xml:space="preserve">Source: 2021-03-23</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: 2021-03-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: 2021-03-09</t>
+    <t xml:space="preserve">Zahl</t>
   </si>
 </sst>
 </file>
@@ -281,15 +284,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J189"/>
+  <dimension ref="A1:J203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H175" activeCellId="0" sqref="H175"/>
+      <selection pane="bottomLeft" activeCell="E200" activeCellId="0" sqref="E200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -3646,12 +3649,6 @@
       <c r="B169" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I169" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J169" s="0" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
@@ -3669,12 +3666,6 @@
       <c r="E170" s="0" t="n">
         <v>6.7</v>
       </c>
-      <c r="I170" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J170" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
@@ -3692,13 +3683,6 @@
       <c r="E171" s="0" t="n">
         <v>9.8</v>
       </c>
-      <c r="I171" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J171" s="0" t="n">
-        <f aca="false">J170 / J169</f>
-        <v>0.384615384615385</v>
-      </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
@@ -3716,12 +3700,6 @@
       <c r="E172" s="0" t="n">
         <v>6.8</v>
       </c>
-      <c r="I172" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J172" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
@@ -3739,12 +3717,6 @@
       <c r="E173" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="I173" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J173" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
@@ -3762,12 +3734,6 @@
       <c r="E174" s="0" t="n">
         <v>7.3</v>
       </c>
-      <c r="I174" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J174" s="3" t="n">
-        <v>11.5</v>
-      </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
@@ -3785,17 +3751,10 @@
       <c r="E175" s="0" t="n">
         <v>11.3</v>
       </c>
-      <c r="I175" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J175" s="1" t="n">
-        <f aca="false">(J174-J172)*J171+J173</f>
-        <v>9.42307692307692</v>
-      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3902,7 +3861,7 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="0" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3921,6 +3880,12 @@
       <c r="E184" s="0" t="n">
         <v>5.6</v>
       </c>
+      <c r="I184" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J184" s="0" t="n">
+        <v>16.75</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
@@ -3936,7 +3901,13 @@
         <v>11250</v>
       </c>
       <c r="E185" s="0" t="n">
-        <v>9.4</v>
+        <v>9.7</v>
+      </c>
+      <c r="I185" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J185" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,6 +3926,13 @@
       <c r="E186" s="0" t="n">
         <v>5.6</v>
       </c>
+      <c r="I186" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J186" s="0" t="n">
+        <f aca="false">J185 / J184</f>
+        <v>0.597014925373134</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
@@ -3972,6 +3950,12 @@
       <c r="E187" s="0" t="n">
         <v>5.5</v>
       </c>
+      <c r="I187" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J187" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
@@ -3989,6 +3973,12 @@
       <c r="E188" s="0" t="n">
         <v>5.7</v>
       </c>
+      <c r="I188" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J188" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
@@ -4005,6 +3995,233 @@
       </c>
       <c r="E189" s="0" t="n">
         <v>7.5</v>
+      </c>
+      <c r="I189" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J189" s="3" t="n">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B190" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J190" s="1" t="n">
+        <f aca="false">(J189-J187)*J186+J188</f>
+        <v>9.44776119402985</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B191" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C191" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D191" s="0" t="n">
+        <v>9333</v>
+      </c>
+      <c r="E191" s="0" t="n">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C192" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" s="0" t="n">
+        <v>14000</v>
+      </c>
+      <c r="E192" s="0" t="n">
+        <v>9.8</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C193" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D193" s="0" t="n">
+        <v>96666</v>
+      </c>
+      <c r="E193" s="0" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C194" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>154000</v>
+      </c>
+      <c r="E194" s="0" t="n">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C195" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" s="0" t="n">
+        <v>86667</v>
+      </c>
+      <c r="E195" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="0" t="n">
+        <v>45000</v>
+      </c>
+      <c r="E196" s="0" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B197" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C198" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D198" s="0" t="n">
+        <v>14000</v>
+      </c>
+      <c r="E198" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B199" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D199" s="0" t="n">
+        <v>19333</v>
+      </c>
+      <c r="E199" s="0" t="n">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B200" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D200" s="0" t="n">
+        <v>102666</v>
+      </c>
+      <c r="E200" s="0" t="n">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B201" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D201" s="0" t="n">
+        <v>156666</v>
+      </c>
+      <c r="E201" s="0" t="n">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B202" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D202" s="0" t="n">
+        <v>88666</v>
+      </c>
+      <c r="E202" s="0" t="n">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B203" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D203" s="0" t="n">
+        <v>45333</v>
+      </c>
+      <c r="E203" s="0" t="n">
+        <v>5.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement vaccinations in the initial conditions and later  (#30)
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="25">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -67,6 +67,12 @@
     <t xml:space="preserve">Source: 2021-02-23</t>
   </si>
   <si>
+    <t xml:space="preserve">Source: 2021-03-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-03-09</t>
+  </si>
+  <si>
     <t xml:space="preserve">Länge für Einheit (cm)</t>
   </si>
   <si>
@@ -85,10 +91,10 @@
     <t xml:space="preserve">Gemessene Höhe (cm)</t>
   </si>
   <si>
-    <t xml:space="preserve">Zahl</t>
+    <t xml:space="preserve">Source: 2021-03-23</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: 2021-03-02</t>
+    <t xml:space="preserve">Zahl</t>
   </si>
 </sst>
 </file>
@@ -278,15 +284,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J182"/>
+  <dimension ref="A1:J203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J171" activeCellId="0" sqref="J171"/>
+      <selection pane="bottomLeft" activeCell="E200" activeCellId="0" sqref="E200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -3643,12 +3649,6 @@
       <c r="B169" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I169" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J169" s="0" t="n">
-        <v>15</v>
-      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
@@ -3666,12 +3666,6 @@
       <c r="E170" s="0" t="n">
         <v>6.7</v>
       </c>
-      <c r="I170" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J170" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
@@ -3689,13 +3683,6 @@
       <c r="E171" s="0" t="n">
         <v>9.8</v>
       </c>
-      <c r="I171" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J171" s="0" t="n">
-        <f aca="false">J170 / J169</f>
-        <v>0.333333333333333</v>
-      </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
@@ -3713,12 +3700,6 @@
       <c r="E172" s="0" t="n">
         <v>6.8</v>
       </c>
-      <c r="I172" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J172" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
@@ -3736,12 +3717,6 @@
       <c r="E173" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="I173" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J173" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
@@ -3759,12 +3734,6 @@
       <c r="E174" s="0" t="n">
         <v>7.3</v>
       </c>
-      <c r="I174" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J174" s="3" t="n">
-        <v>3.6</v>
-      </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
@@ -3782,17 +3751,10 @@
       <c r="E175" s="0" t="n">
         <v>11.3</v>
       </c>
-      <c r="I175" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J175" s="1" t="n">
-        <f aca="false">(J174-J172)*J171+J173</f>
-        <v>6.2</v>
-      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3895,6 +3857,371 @@
       </c>
       <c r="E182" s="0" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B183" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D184" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="E184" s="0" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="I184" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J184" s="0" t="n">
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D185" s="0" t="n">
+        <v>11250</v>
+      </c>
+      <c r="E185" s="0" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="I185" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J185" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C186" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D186" s="0" t="n">
+        <v>93750</v>
+      </c>
+      <c r="E186" s="0" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="I186" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J186" s="0" t="n">
+        <f aca="false">J185 / J184</f>
+        <v>0.597014925373134</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C187" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>150000</v>
+      </c>
+      <c r="E187" s="0" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="I187" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J187" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C188" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D188" s="0" t="n">
+        <v>84750</v>
+      </c>
+      <c r="E188" s="0" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="I188" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J188" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C189" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D189" s="0" t="n">
+        <v>46500</v>
+      </c>
+      <c r="E189" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I189" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J189" s="3" t="n">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B190" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J190" s="1" t="n">
+        <f aca="false">(J189-J187)*J186+J188</f>
+        <v>9.44776119402985</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B191" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C191" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D191" s="0" t="n">
+        <v>9333</v>
+      </c>
+      <c r="E191" s="0" t="n">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C192" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" s="0" t="n">
+        <v>14000</v>
+      </c>
+      <c r="E192" s="0" t="n">
+        <v>9.8</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C193" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D193" s="0" t="n">
+        <v>96666</v>
+      </c>
+      <c r="E193" s="0" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C194" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>154000</v>
+      </c>
+      <c r="E194" s="0" t="n">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C195" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" s="0" t="n">
+        <v>86667</v>
+      </c>
+      <c r="E195" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="0" t="n">
+        <v>45000</v>
+      </c>
+      <c r="E196" s="0" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B197" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C198" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D198" s="0" t="n">
+        <v>14000</v>
+      </c>
+      <c r="E198" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B199" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D199" s="0" t="n">
+        <v>19333</v>
+      </c>
+      <c r="E199" s="0" t="n">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B200" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D200" s="0" t="n">
+        <v>102666</v>
+      </c>
+      <c r="E200" s="0" t="n">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B201" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D201" s="0" t="n">
+        <v>156666</v>
+      </c>
+      <c r="E201" s="0" t="n">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B202" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D202" s="0" t="n">
+        <v>88666</v>
+      </c>
+      <c r="E202" s="0" t="n">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B203" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D203" s="0" t="n">
+        <v>45333</v>
+      </c>
+      <c r="E203" s="0" t="n">
+        <v>5.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ARS and virus strain data (#40)
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="26">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-02-30</t>
   </si>
 </sst>
 </file>
@@ -284,15 +287,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J203"/>
+  <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E200" activeCellId="0" sqref="E200"/>
+      <selection pane="bottomLeft" activeCell="E215" activeCellId="0" sqref="E215"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -4224,6 +4227,215 @@
         <v>5.3</v>
       </c>
     </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B204" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B205" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" s="0" t="n">
+        <v>18750</v>
+      </c>
+      <c r="E205" s="0" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D206" s="0" t="n">
+        <v>28009</v>
+      </c>
+      <c r="E206" s="0" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B207" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D207" s="0" t="n">
+        <v>108796</v>
+      </c>
+      <c r="E207" s="0" t="n">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B208" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D208" s="0" t="n">
+        <v>161342</v>
+      </c>
+      <c r="E208" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B209" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D209" s="0" t="n">
+        <v>89815</v>
+      </c>
+      <c r="E209" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B210" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D210" s="0" t="n">
+        <v>44444</v>
+      </c>
+      <c r="E210" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B212" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D212" s="0" t="n">
+        <v>28472</v>
+      </c>
+      <c r="E212" s="0" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B213" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D213" s="0" t="n">
+        <v>41666</v>
+      </c>
+      <c r="E213" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B214" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D214" s="0" t="n">
+        <v>119444</v>
+      </c>
+      <c r="E214" s="0" t="n">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B215" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D215" s="0" t="n">
+        <v>170601</v>
+      </c>
+      <c r="E215" s="0" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B216" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C216" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D216" s="0" t="n">
+        <v>91890</v>
+      </c>
+      <c r="E216" s="0" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B217" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D217" s="0" t="n">
+        <v>44444</v>
+      </c>
+      <c r="E217" s="0" t="n">
+        <v>5.2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
new share_known_cases, make susceptibility age_dependent, start on new estimation notebook, speed up, recurrent boolean columns (#36)
Co-authored-by: Klara Roehrl <klara.roehrl@gmail.com>
Co-authored-by: Tobias Raabe <raabe@posteo.de>
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="26">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-02-30</t>
   </si>
 </sst>
 </file>
@@ -284,15 +287,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J203"/>
+  <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E200" activeCellId="0" sqref="E200"/>
+      <selection pane="bottomLeft" activeCell="E215" activeCellId="0" sqref="E215"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -4224,6 +4227,215 @@
         <v>5.3</v>
       </c>
     </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B204" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B205" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" s="0" t="n">
+        <v>18750</v>
+      </c>
+      <c r="E205" s="0" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D206" s="0" t="n">
+        <v>28009</v>
+      </c>
+      <c r="E206" s="0" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B207" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D207" s="0" t="n">
+        <v>108796</v>
+      </c>
+      <c r="E207" s="0" t="n">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B208" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D208" s="0" t="n">
+        <v>161342</v>
+      </c>
+      <c r="E208" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B209" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D209" s="0" t="n">
+        <v>89815</v>
+      </c>
+      <c r="E209" s="0" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B210" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D210" s="0" t="n">
+        <v>44444</v>
+      </c>
+      <c r="E210" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B212" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D212" s="0" t="n">
+        <v>28472</v>
+      </c>
+      <c r="E212" s="0" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B213" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D213" s="0" t="n">
+        <v>41666</v>
+      </c>
+      <c r="E213" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B214" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D214" s="0" t="n">
+        <v>119444</v>
+      </c>
+      <c r="E214" s="0" t="n">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B215" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D215" s="0" t="n">
+        <v>170601</v>
+      </c>
+      <c r="E215" s="0" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B216" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C216" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D216" s="0" t="n">
+        <v>91890</v>
+      </c>
+      <c r="E216" s="0" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B217" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D217" s="0" t="n">
+        <v>44444</v>
+      </c>
+      <c r="E217" s="0" t="n">
+        <v>5.2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add new testing data by ARS and update the cologne virus variant data. (#44)
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="28">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -97,7 +97,13 @@
     <t xml:space="preserve">Zahl</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: 2021-02-30</t>
+    <t xml:space="preserve">Source: 2021-03-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-04-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAREFUL EASTER WEEK</t>
   </si>
 </sst>
 </file>
@@ -193,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,6 +214,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -287,15 +297,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:J225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E215" activeCellId="0" sqref="E215"/>
+      <selection pane="bottomLeft" activeCell="E222" activeCellId="0" sqref="E222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -4334,6 +4344,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B211" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="n">
         <v>2021</v>
@@ -4345,10 +4360,10 @@
         <v>7</v>
       </c>
       <c r="D212" s="0" t="n">
-        <v>28472</v>
+        <v>28603</v>
       </c>
       <c r="E212" s="0" t="n">
-        <v>5.1</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4362,10 +4377,10 @@
         <v>8</v>
       </c>
       <c r="D213" s="0" t="n">
-        <v>41666</v>
+        <v>41242</v>
       </c>
       <c r="E213" s="0" t="n">
-        <v>8</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4379,10 +4394,10 @@
         <v>9</v>
       </c>
       <c r="D214" s="0" t="n">
-        <v>119444</v>
+        <v>119401</v>
       </c>
       <c r="E214" s="0" t="n">
-        <v>8.6</v>
+        <v>8.8</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4399,7 +4414,7 @@
         <v>170601</v>
       </c>
       <c r="E215" s="0" t="n">
-        <v>8.5</v>
+        <v>8.7</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4413,10 +4428,10 @@
         <v>11</v>
       </c>
       <c r="D216" s="0" t="n">
-        <v>91890</v>
+        <v>90798</v>
       </c>
       <c r="E216" s="0" t="n">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4430,10 +4445,117 @@
         <v>12</v>
       </c>
       <c r="D217" s="0" t="n">
-        <v>44444</v>
+        <v>43902</v>
       </c>
       <c r="E217" s="0" t="n">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B219" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D219" s="0" t="n">
+        <v>28271</v>
+      </c>
+      <c r="E219" s="0" t="n">
         <v>5.2</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B220" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C220" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D220" s="0" t="n">
+        <v>45898</v>
+      </c>
+      <c r="E220" s="0" t="n">
+        <v>8.2</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B221" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C221" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D221" s="0" t="n">
+        <v>129379</v>
+      </c>
+      <c r="E221" s="0" t="n">
+        <v>8.8</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B222" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C222" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D222" s="0" t="n">
+        <v>184590</v>
+      </c>
+      <c r="E222" s="0" t="n">
+        <v>8.7</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B223" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D223" s="0" t="n">
+        <v>93459</v>
+      </c>
+      <c r="E223" s="0" t="n">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B224" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C224" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D224" s="0" t="n">
+        <v>45898</v>
+      </c>
+      <c r="E224" s="0" t="n">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B225" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ARS data. (#50)
</commit_message>
<xml_diff>
--- a/src/original_data/testing/ars_data_raw.xlsx
+++ b/src/original_data/testing/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="27">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -100,10 +100,7 @@
     <t xml:space="preserve">Source: 2021-03-30</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: 2021-04-06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAREFUL EASTER WEEK</t>
+    <t xml:space="preserve">Source: 2021-04-13</t>
   </si>
 </sst>
 </file>
@@ -216,7 +213,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,15 +294,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J225"/>
+  <dimension ref="A1:J231"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E222" activeCellId="0" sqref="E222"/>
+      <selection pane="bottomLeft" activeCell="E228" activeCellId="0" sqref="E228"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -4360,7 +4357,7 @@
         <v>7</v>
       </c>
       <c r="D212" s="0" t="n">
-        <v>28603</v>
+        <v>28748</v>
       </c>
       <c r="E212" s="0" t="n">
         <v>5.2</v>
@@ -4377,10 +4374,10 @@
         <v>8</v>
       </c>
       <c r="D213" s="0" t="n">
-        <v>41242</v>
+        <v>42125</v>
       </c>
       <c r="E213" s="0" t="n">
-        <v>8.1</v>
+        <v>8.2</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,7 +4391,7 @@
         <v>9</v>
       </c>
       <c r="D214" s="0" t="n">
-        <v>119401</v>
+        <v>119829</v>
       </c>
       <c r="E214" s="0" t="n">
         <v>8.8</v>
@@ -4411,10 +4408,10 @@
         <v>10</v>
       </c>
       <c r="D215" s="0" t="n">
-        <v>170601</v>
+        <v>172201</v>
       </c>
       <c r="E215" s="0" t="n">
-        <v>8.7</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4428,10 +4425,10 @@
         <v>11</v>
       </c>
       <c r="D216" s="0" t="n">
-        <v>90798</v>
+        <v>91935</v>
       </c>
       <c r="E216" s="0" t="n">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4445,10 +4442,10 @@
         <v>12</v>
       </c>
       <c r="D217" s="0" t="n">
-        <v>43902</v>
+        <v>44687</v>
       </c>
       <c r="E217" s="0" t="n">
-        <v>5.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4462,10 +4459,10 @@
         <v>7</v>
       </c>
       <c r="D219" s="0" t="n">
-        <v>28271</v>
+        <v>27609</v>
       </c>
       <c r="E219" s="0" t="n">
-        <v>5.2</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4479,10 +4476,10 @@
         <v>8</v>
       </c>
       <c r="D220" s="0" t="n">
-        <v>45898</v>
+        <v>47250</v>
       </c>
       <c r="E220" s="0" t="n">
-        <v>8.2</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4496,10 +4493,10 @@
         <v>9</v>
       </c>
       <c r="D221" s="0" t="n">
-        <v>129379</v>
+        <v>131500</v>
       </c>
       <c r="E221" s="0" t="n">
-        <v>8.8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4513,10 +4510,10 @@
         <v>10</v>
       </c>
       <c r="D222" s="0" t="n">
-        <v>184590</v>
+        <v>187287</v>
       </c>
       <c r="E222" s="0" t="n">
-        <v>8.7</v>
+        <v>9.8</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4530,10 +4527,10 @@
         <v>11</v>
       </c>
       <c r="D223" s="0" t="n">
-        <v>93459</v>
+        <v>95351</v>
       </c>
       <c r="E223" s="0" t="n">
-        <v>6.8</v>
+        <v>8</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4547,15 +4544,115 @@
         <v>12</v>
       </c>
       <c r="D224" s="0" t="n">
-        <v>45898</v>
+        <v>46395</v>
       </c>
       <c r="E224" s="0" t="n">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="4" t="s">
-        <v>27</v>
+      <c r="B225" s="4"/>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B226" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C226" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D226" s="0" t="n">
+        <v>21632</v>
+      </c>
+      <c r="E226" s="0" t="n">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B227" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D227" s="0" t="n">
+        <v>30455</v>
+      </c>
+      <c r="E227" s="0" t="n">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B228" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D228" s="0" t="n">
+        <v>107306</v>
+      </c>
+      <c r="E228" s="0" t="n">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B229" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C229" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D229" s="0" t="n">
+        <v>151992</v>
+      </c>
+      <c r="E229" s="0" t="n">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B230" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C230" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D230" s="0" t="n">
+        <v>77135</v>
+      </c>
+      <c r="E230" s="0" t="n">
+        <v>9.7</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B231" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C231" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D231" s="0" t="n">
+        <v>38994</v>
+      </c>
+      <c r="E231" s="0" t="n">
+        <v>6.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>